<commit_message>
[B3] PT re-test + CPT 서식수정
PT Iter#1 re-test 결과와 CPT 테스트결과 일부 서식 수정
</commit_message>
<xml_diff>
--- a/combinatorial/test exec/combinatorial 테스트결과 B3.xlsx
+++ b/combinatorial/test exec/combinatorial 테스트결과 B3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyGGit\vnv-team-3\combinatorial\test exec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08781E9A-C380-4EA0-98C6-045DABD6EC14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB30F17B-3BB2-4FAD-86A4-B3E51681C4AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="테스트케이스 포맷" sheetId="1" r:id="rId1"/>
@@ -308,10 +308,6 @@
     <t>selected mode number &gt;= 5</t>
   </si>
   <si>
-    <t>Iter#2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Iter#1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -339,6 +335,10 @@
   </si>
   <si>
     <t>iter #1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Re-test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -346,7 +346,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,6 +385,13 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Raleway"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="9"/>
       <name val="Raleway"/>
       <family val="2"/>
     </font>
@@ -569,15 +576,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -592,13 +590,22 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -881,7 +888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -897,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA991DCF-D0C7-493C-9A0A-83C276513055}">
   <dimension ref="C5:J65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -911,43 +918,43 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:10" ht="18" thickBot="1">
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" ht="18" thickBot="1">
+      <c r="I6" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J6" s="18"/>
+    </row>
+    <row r="7" spans="3:10">
+      <c r="C7" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="J7" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="3:10" ht="18" thickBot="1">
-      <c r="I6" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="J6" s="17"/>
-    </row>
-    <row r="7" spans="3:10" ht="26.4">
-      <c r="C7" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10" ht="52.8">
+    <row r="8" spans="3:10">
       <c r="C8" s="6">
         <v>1</v>
       </c>
@@ -973,7 +980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="3:10" ht="26.4">
+    <row r="9" spans="3:10">
       <c r="C9" s="6">
         <v>2</v>
       </c>
@@ -999,7 +1006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="3:10" ht="26.4">
+    <row r="10" spans="3:10">
       <c r="C10" s="6">
         <v>3</v>
       </c>
@@ -1025,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="3:10" ht="26.4">
+    <row r="11" spans="3:10">
       <c r="C11" s="6">
         <v>4</v>
       </c>
@@ -1051,7 +1058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="3:10" ht="26.4">
+    <row r="12" spans="3:10">
       <c r="C12" s="6">
         <v>5</v>
       </c>
@@ -1077,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="3:10" ht="26.4">
+    <row r="13" spans="3:10">
       <c r="C13" s="6">
         <v>6</v>
       </c>
@@ -1103,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:10" ht="26.4">
+    <row r="14" spans="3:10">
       <c r="C14" s="6">
         <v>7</v>
       </c>
@@ -1129,7 +1136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:10" ht="26.4">
+    <row r="15" spans="3:10">
       <c r="C15" s="6">
         <v>8</v>
       </c>
@@ -1155,7 +1162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="3:10" ht="26.4">
+    <row r="16" spans="3:10">
       <c r="C16" s="6">
         <v>9</v>
       </c>
@@ -1181,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:10" ht="26.4">
+    <row r="17" spans="3:10">
       <c r="C17" s="6">
         <v>10</v>
       </c>
@@ -1207,7 +1214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:10" ht="26.4">
+    <row r="18" spans="3:10">
       <c r="C18" s="6">
         <v>11</v>
       </c>
@@ -1233,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:10" ht="26.4">
+    <row r="19" spans="3:10">
       <c r="C19" s="6">
         <v>12</v>
       </c>
@@ -1259,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:10" ht="26.4">
+    <row r="20" spans="3:10">
       <c r="C20" s="6">
         <v>13</v>
       </c>
@@ -1285,7 +1292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:10" ht="26.4">
+    <row r="21" spans="3:10">
       <c r="C21" s="6">
         <v>14</v>
       </c>
@@ -1311,7 +1318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:10" ht="26.4">
+    <row r="22" spans="3:10">
       <c r="C22" s="6">
         <v>15</v>
       </c>
@@ -1337,7 +1344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:10" ht="26.4">
+    <row r="23" spans="3:10">
       <c r="C23" s="6">
         <v>16</v>
       </c>
@@ -1363,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:10" ht="26.4">
+    <row r="24" spans="3:10">
       <c r="C24" s="6">
         <v>17</v>
       </c>
@@ -1389,7 +1396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:10" ht="26.4">
+    <row r="25" spans="3:10">
       <c r="C25" s="6">
         <v>18</v>
       </c>
@@ -1415,7 +1422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:10" ht="26.4">
+    <row r="26" spans="3:10">
       <c r="C26" s="6">
         <v>19</v>
       </c>
@@ -1441,57 +1448,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:10" ht="27" thickBot="1">
-      <c r="C27" s="13">
+    <row r="27" spans="3:10" ht="18" thickBot="1">
+      <c r="C27" s="10">
         <v>20</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H27" s="12" t="s">
+      <c r="G27" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="I27" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J27" s="10" t="s">
+      <c r="J27" s="19" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="3:10" ht="18" thickTop="1">
       <c r="C28" s="6"/>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
       <c r="J28" s="7"/>
     </row>
     <row r="29" spans="3:10">
       <c r="C29" s="6"/>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="3:10" ht="26.4">
+    <row r="30" spans="3:10">
       <c r="C30" s="6">
         <v>21</v>
       </c>
@@ -1517,57 +1524,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:10" ht="27" thickBot="1">
-      <c r="C31" s="13">
+    <row r="31" spans="3:10" ht="18" thickBot="1">
+      <c r="C31" s="10">
         <v>22</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="G31" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H31" s="12" t="s">
+      <c r="G31" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H31" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I31" s="11" t="s">
+      <c r="I31" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J31" s="10" t="s">
+      <c r="J31" s="19" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="3:10" ht="18" thickTop="1">
       <c r="C32" s="6"/>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
       <c r="J32" s="7"/>
     </row>
     <row r="33" spans="3:10">
       <c r="C33" s="6"/>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
       <c r="J33" s="7"/>
     </row>
-    <row r="34" spans="3:10" ht="26.4">
+    <row r="34" spans="3:10">
       <c r="C34" s="6">
         <v>23</v>
       </c>
@@ -1593,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:10" ht="26.4">
+    <row r="35" spans="3:10">
       <c r="C35" s="6">
         <v>24</v>
       </c>
@@ -1619,7 +1626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:10" ht="26.4">
+    <row r="36" spans="3:10">
       <c r="C36" s="6">
         <v>25</v>
       </c>
@@ -1645,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:10" ht="26.4">
+    <row r="37" spans="3:10">
       <c r="C37" s="6">
         <v>26</v>
       </c>
@@ -1671,7 +1678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:10" ht="26.4">
+    <row r="38" spans="3:10">
       <c r="C38" s="6">
         <v>27</v>
       </c>
@@ -1697,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:10" ht="26.4">
+    <row r="39" spans="3:10">
       <c r="C39" s="6">
         <v>28</v>
       </c>
@@ -1723,7 +1730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:10" ht="26.4">
+    <row r="40" spans="3:10">
       <c r="C40" s="6">
         <v>29</v>
       </c>
@@ -1749,7 +1756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:10" ht="26.4">
+    <row r="41" spans="3:10">
       <c r="C41" s="6">
         <v>30</v>
       </c>
@@ -1775,7 +1782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:10" ht="26.4">
+    <row r="42" spans="3:10">
       <c r="C42" s="6">
         <v>31</v>
       </c>
@@ -1827,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:10" ht="26.4">
+    <row r="44" spans="3:10">
       <c r="C44" s="6">
         <v>33</v>
       </c>
@@ -1853,7 +1860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:10" ht="26.4">
+    <row r="45" spans="3:10">
       <c r="C45" s="6">
         <v>34</v>
       </c>
@@ -1905,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:10" ht="39.6">
+    <row r="47" spans="3:10">
       <c r="C47" s="6">
         <v>36</v>
       </c>
@@ -1931,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:10" ht="26.4">
+    <row r="48" spans="3:10">
       <c r="C48" s="6">
         <v>37</v>
       </c>
@@ -1957,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:10" ht="26.4">
+    <row r="49" spans="3:10">
       <c r="C49" s="6">
         <v>38</v>
       </c>
@@ -1983,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="3:10" ht="26.4">
+    <row r="50" spans="3:10">
       <c r="C50" s="6">
         <v>39</v>
       </c>
@@ -2009,7 +2016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="3:10" ht="26.4">
+    <row r="51" spans="3:10">
       <c r="C51" s="6">
         <v>40</v>
       </c>
@@ -2035,7 +2042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="3:10" ht="26.4">
+    <row r="52" spans="3:10">
       <c r="C52" s="6">
         <v>41</v>
       </c>
@@ -2061,7 +2068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="3:10" ht="26.4">
+    <row r="53" spans="3:10">
       <c r="C53" s="6">
         <v>42</v>
       </c>
@@ -2087,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:10" ht="26.4">
+    <row r="54" spans="3:10">
       <c r="C54" s="6">
         <v>43</v>
       </c>
@@ -2113,7 +2120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="3:10" ht="26.4">
+    <row r="55" spans="3:10">
       <c r="C55" s="6">
         <v>44</v>
       </c>
@@ -2139,7 +2146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="3:10" ht="26.4">
+    <row r="56" spans="3:10">
       <c r="C56" s="6">
         <v>45</v>
       </c>
@@ -2165,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:10" ht="26.4">
+    <row r="57" spans="3:10">
       <c r="C57" s="6">
         <v>46</v>
       </c>
@@ -2191,7 +2198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="3:10" ht="26.4">
+    <row r="58" spans="3:10">
       <c r="C58" s="6">
         <v>47</v>
       </c>
@@ -2217,7 +2224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="3:10" ht="26.4">
+    <row r="59" spans="3:10">
       <c r="C59" s="6">
         <v>48</v>
       </c>
@@ -2243,7 +2250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="3:10" ht="26.4">
+    <row r="60" spans="3:10">
       <c r="C60" s="6">
         <v>49</v>
       </c>
@@ -2269,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="3:10" ht="26.4">
+    <row r="61" spans="3:10">
       <c r="C61" s="6">
         <v>50</v>
       </c>
@@ -2295,7 +2302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="3:10" ht="26.4">
+    <row r="62" spans="3:10">
       <c r="C62" s="6">
         <v>51</v>
       </c>
@@ -2321,7 +2328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="3:10" ht="26.4">
+    <row r="63" spans="3:10">
       <c r="C63" s="6">
         <v>52</v>
       </c>
@@ -2347,7 +2354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="3:10" ht="26.4">
+    <row r="64" spans="3:10">
       <c r="C64" s="6">
         <v>53</v>
       </c>
@@ -2373,7 +2380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="3:10" ht="27" thickBot="1">
+    <row r="65" spans="3:10" ht="18" thickBot="1">
       <c r="C65" s="3">
         <v>54</v>
       </c>
@@ -2409,5 +2416,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>